<commit_message>
Amended battery config spreadsheet with new graphics
</commit_message>
<xml_diff>
--- a/Hardware/Batteries/Pijuice_battery_config.xlsx
+++ b/Hardware/Batteries/Pijuice_battery_config.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="22280" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Dip switch" sheetId="4" r:id="rId1"/>
     <sheet name="Profile selection" sheetId="3" r:id="rId2"/>
     <sheet name="Charge settings" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -127,16 +132,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -169,6 +174,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -306,14 +319,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -329,28 +334,28 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>25401</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
+      <xdr:colOff>719954</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>472312</xdr:rowOff>
+      <xdr:rowOff>749300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Dip-10-BP7X.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -363,8 +368,122 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6416040" y="373380"/>
-          <a:ext cx="495300" cy="464692"/>
+          <a:off x="9766301" y="939800"/>
+          <a:ext cx="694553" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>732137</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>762000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9766299" y="2552700"/>
+          <a:ext cx="706738" cy="736600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>779351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="1765300"/>
+          <a:ext cx="711200" cy="741251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>713166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="228599"/>
+          <a:ext cx="647700" cy="675067"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -380,12 +499,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0">
   <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Profile code" dataDxfId="5"/>
-    <tableColumn id="2" name="Battery profile name" dataDxfId="4"/>
-    <tableColumn id="3" name="Switch position 1" dataDxfId="3"/>
-    <tableColumn id="4" name="Switch position 2" dataDxfId="2"/>
-    <tableColumn id="5" name="Switch code" dataDxfId="1"/>
-    <tableColumn id="6" name="Example" dataDxfId="0"/>
+    <tableColumn id="1" name="Profile code" dataDxfId="7"/>
+    <tableColumn id="2" name="Battery profile name" dataDxfId="6"/>
+    <tableColumn id="3" name="Switch position 1" dataDxfId="5"/>
+    <tableColumn id="4" name="Switch position 2" dataDxfId="4"/>
+    <tableColumn id="5" name="Switch code" dataDxfId="3"/>
+    <tableColumn id="6" name="Example" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -398,7 +517,7 @@
     <tableColumn id="1" name="Profile code"/>
     <tableColumn id="2" name="Battery profile name"/>
     <tableColumn id="3" name="R [Kohm]"/>
-    <tableColumn id="4" name="Dip switch" dataDxfId="6"/>
+    <tableColumn id="4" name="Dip switch" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,7 +529,7 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Settings code"/>
     <tableColumn id="2" name="R [KOhm]"/>
-    <tableColumn id="3" name="Dip switch" dataDxfId="7"/>
+    <tableColumn id="3" name="Dip switch" dataDxfId="0"/>
     <tableColumn id="4" name="Charge current [mA]"/>
     <tableColumn id="5" name="Termination current [mA]"/>
     <tableColumn id="6" name="Regulation voltage [V]"/>
@@ -462,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -709,19 +828,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.75" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -741,7 +860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="57" customHeight="1">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -759,7 +878,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="64" customHeight="1">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -777,7 +896,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="63" customHeight="1">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -795,7 +914,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="61" customHeight="1">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -815,11 +934,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -831,15 +955,15 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -853,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -867,7 +991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -881,7 +1005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -895,7 +1019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -909,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -920,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -931,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -942,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -953,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -964,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -975,7 +1099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -986,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>11</v>
       </c>
@@ -997,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1008,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1019,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1030,7 +1154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1046,6 +1170,11 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1057,18 +1186,18 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="21.25" customWidth="1"/>
+    <col min="5" max="5" width="24.75" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1108,7 +1237,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1128,7 +1257,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1148,7 +1277,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1168,7 +1297,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1188,7 +1317,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1208,7 +1337,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1228,7 +1357,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1248,7 +1377,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1268,7 +1397,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1288,7 +1417,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1308,7 +1437,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1328,7 +1457,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1348,7 +1477,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1368,7 +1497,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1388,7 +1517,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1408,7 +1537,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1428,7 +1557,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1448,7 +1577,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1468,7 +1597,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1488,7 +1617,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1508,7 +1637,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1528,7 +1657,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1548,7 +1677,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1568,7 +1697,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1588,7 +1717,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1608,7 +1737,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1628,7 +1757,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1648,7 +1777,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1668,7 +1797,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1688,7 +1817,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1708,7 +1837,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1728,7 +1857,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1748,7 +1877,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1768,7 +1897,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1788,7 +1917,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1808,7 +1937,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1828,7 +1957,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1848,7 +1977,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1868,7 +1997,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1888,7 +2017,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1908,7 +2037,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1928,7 +2057,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1948,7 +2077,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1968,7 +2097,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1988,7 +2117,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2008,7 +2137,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2028,7 +2157,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2048,7 +2177,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2068,7 +2197,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2088,7 +2217,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2108,7 +2237,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2128,7 +2257,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2148,7 +2277,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2168,7 +2297,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2188,7 +2317,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2208,7 +2337,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2228,7 +2357,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2248,7 +2377,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2268,7 +2397,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2288,7 +2417,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2308,7 +2437,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2328,7 +2457,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2348,7 +2477,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2368,7 +2497,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2388,7 +2517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2408,7 +2537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2428,7 +2557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2448,7 +2577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2468,7 +2597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2488,7 +2617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2508,7 +2637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2528,7 +2657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2548,7 +2677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2568,7 +2697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2588,7 +2717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2608,7 +2737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2628,7 +2757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2648,7 +2777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2668,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2688,7 +2817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2708,7 +2837,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2728,7 +2857,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2748,7 +2877,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2768,7 +2897,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2788,7 +2917,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2808,7 +2937,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2828,7 +2957,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2848,7 +2977,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2868,7 +2997,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6">
       <c r="A91">
         <v>89</v>
       </c>
@@ -2888,7 +3017,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2908,7 +3037,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6">
       <c r="A93">
         <v>91</v>
       </c>
@@ -2928,7 +3057,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6">
       <c r="A94">
         <v>92</v>
       </c>
@@ -2948,7 +3077,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6">
       <c r="A95">
         <v>93</v>
       </c>
@@ -2968,7 +3097,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6">
       <c r="A96">
         <v>94</v>
       </c>
@@ -2988,7 +3117,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3008,7 +3137,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3028,7 +3157,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3048,7 +3177,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3068,7 +3197,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3088,7 +3217,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3108,7 +3237,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3128,7 +3257,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3148,7 +3277,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3168,7 +3297,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6">
       <c r="A106">
         <v>104</v>
       </c>
@@ -3188,7 +3317,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6">
       <c r="A107">
         <v>105</v>
       </c>
@@ -3208,7 +3337,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6">
       <c r="A108">
         <v>106</v>
       </c>
@@ -3228,7 +3357,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3248,7 +3377,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3268,7 +3397,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6">
       <c r="A111">
         <v>109</v>
       </c>
@@ -3288,7 +3417,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6">
       <c r="A112">
         <v>110</v>
       </c>
@@ -3308,7 +3437,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6">
       <c r="A113">
         <v>111</v>
       </c>
@@ -3328,7 +3457,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6">
       <c r="A114">
         <v>112</v>
       </c>
@@ -3348,7 +3477,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6">
       <c r="A115">
         <v>113</v>
       </c>
@@ -3368,7 +3497,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6">
       <c r="A116">
         <v>114</v>
       </c>
@@ -3388,7 +3517,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6">
       <c r="A117">
         <v>115</v>
       </c>
@@ -3408,7 +3537,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6">
       <c r="A118">
         <v>116</v>
       </c>
@@ -3428,7 +3557,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6">
       <c r="A119">
         <v>117</v>
       </c>
@@ -3448,7 +3577,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6">
       <c r="A120">
         <v>118</v>
       </c>
@@ -3468,7 +3597,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6">
       <c r="A121">
         <v>119</v>
       </c>
@@ -3488,7 +3617,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6">
       <c r="A122">
         <v>120</v>
       </c>
@@ -3508,7 +3637,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6">
       <c r="A123">
         <v>121</v>
       </c>
@@ -3528,7 +3657,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6">
       <c r="A124">
         <v>122</v>
       </c>
@@ -3548,7 +3677,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6">
       <c r="A125">
         <v>123</v>
       </c>
@@ -3568,7 +3697,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6">
       <c r="A126">
         <v>124</v>
       </c>
@@ -3588,7 +3717,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6">
       <c r="A127">
         <v>125</v>
       </c>
@@ -3608,7 +3737,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6">
       <c r="A128">
         <v>126</v>
       </c>
@@ -3628,7 +3757,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6">
       <c r="A129">
         <v>127</v>
       </c>
@@ -3650,9 +3779,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amended battery config spreadsheet with additional example Added software install manual steps
</commit_message>
<xml_diff>
--- a/Hardware/Batteries/Pijuice_battery_config.xlsx
+++ b/Hardware/Batteries/Pijuice_battery_config.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="22280" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dip switch" sheetId="4" r:id="rId1"/>
     <sheet name="Profile selection" sheetId="3" r:id="rId2"/>
     <sheet name="Charge settings" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171026" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,18 +21,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="25">
+  <si>
+    <t>Profile code</t>
+  </si>
+  <si>
+    <t>Battery profile name</t>
+  </si>
+  <si>
+    <t>Switch position 1</t>
+  </si>
+  <si>
+    <t>Switch position 2</t>
+  </si>
+  <si>
+    <t>Switch positions in binary</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Switch code (for use in firmware only)</t>
+  </si>
+  <si>
+    <t>BP6X</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>BP7X</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>SNN5843  2300mAh</t>
+  </si>
+  <si>
+    <t>LIPO8047109  5000mAh</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
   <si>
     <t>R [Kohm]</t>
-  </si>
-  <si>
-    <t>R [KOhm]</t>
   </si>
   <si>
     <t>Dip switch</t>
   </si>
   <si>
-    <t>01</t>
+    <t>Settings code</t>
+  </si>
+  <si>
+    <t>R [KOhm]</t>
   </si>
   <si>
     <t>Charge current [mA]</t>
@@ -44,63 +95,26 @@
     <t>Regulation voltage [V]</t>
   </si>
   <si>
-    <t>Settings code</t>
-  </si>
-  <si>
-    <t>Profile code</t>
-  </si>
-  <si>
-    <t>Battery profile name</t>
-  </si>
-  <si>
-    <t>BP6X</t>
-  </si>
-  <si>
-    <t>BP7X</t>
-  </si>
-  <si>
-    <t>SNN5843  2300mAh</t>
-  </si>
-  <si>
-    <t>LIPO8047109  5000mAh</t>
-  </si>
-  <si>
-    <t>Switch position 1</t>
-  </si>
-  <si>
-    <t>Switch code</t>
-  </si>
-  <si>
-    <t>Switch position 2</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>Example</t>
+    <t>DIP Switch Location "01" is as shown above (same as default / BP7X setting)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -167,6 +181,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -209,23 +228,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -337,19 +352,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>25401</xdr:colOff>
+      <xdr:colOff>53976</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>719954</xdr:colOff>
+      <xdr:colOff>748529</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>749300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Dip-10-BP7X.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Dip-10-BP7X.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -368,7 +389,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9766301" y="939800"/>
+          <a:off x="8940801" y="939800"/>
           <a:ext cx="694553" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -381,19 +402,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>25399</xdr:colOff>
+      <xdr:colOff>44449</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>732137</xdr:colOff>
+      <xdr:colOff>751187</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>762000</xdr:rowOff>
+      <xdr:rowOff>752475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -406,7 +436,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9766299" y="2552700"/>
+          <a:off x="8931274" y="2540000"/>
           <a:ext cx="706738" cy="736600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -419,19 +449,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:colOff>758825</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>779351</xdr:rowOff>
+      <xdr:rowOff>760301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -444,7 +483,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9779000" y="1765300"/>
+          <a:off x="8934450" y="1743075"/>
           <a:ext cx="711200" cy="741251"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -457,19 +496,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>733425</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>713166</xdr:rowOff>
+      <xdr:rowOff>694116</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -482,7 +530,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9779000" y="228599"/>
+          <a:off x="8972550" y="209549"/>
           <a:ext cx="647700" cy="675067"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -495,44 +543,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123053</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Dip-10-BP7X.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{133534F5-0341-46FD-AD2A-11BAA6269D24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="190500"/>
+          <a:ext cx="694553" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Profile code" dataDxfId="7"/>
-    <tableColumn id="2" name="Battery profile name" dataDxfId="6"/>
-    <tableColumn id="3" name="Switch position 1" dataDxfId="5"/>
-    <tableColumn id="4" name="Switch position 2" dataDxfId="4"/>
-    <tableColumn id="5" name="Switch code" dataDxfId="3"/>
-    <tableColumn id="6" name="Example" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Profile code" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Battery profile name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Switch position 1" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Switch position 2" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{A155D7C2-CE3E-4107-B898-0450854CCA64}" name="Switch positions in binary" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Example" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Profile code"/>
-    <tableColumn id="2" name="Battery profile name"/>
-    <tableColumn id="3" name="R [Kohm]"/>
-    <tableColumn id="4" name="Dip switch" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Profile code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Battery profile name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="R [Kohm]"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Dip switch" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F129" totalsRowShown="0">
-  <autoFilter ref="A1:F129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:F129" totalsRowShown="0">
+  <autoFilter ref="A1:F129" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Settings code"/>
-    <tableColumn id="2" name="R [KOhm]"/>
-    <tableColumn id="3" name="Dip switch" dataDxfId="0"/>
-    <tableColumn id="4" name="Charge current [mA]"/>
-    <tableColumn id="5" name="Termination current [mA]"/>
-    <tableColumn id="6" name="Regulation voltage [V]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Settings code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="R [KOhm]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Dip switch" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Charge current [mA]"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Termination current [mA]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Regulation voltage [V]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,113 +927,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="26.75" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="57" customHeight="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="64" customHeight="1">
+      <c r="G2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="63" customHeight="1">
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="61" customHeight="1">
+    </row>
+    <row r="5" spans="1:7" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7"/>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,92 +1067,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>23.5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>22.6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1041,10 +1160,13 @@
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1052,10 +1174,10 @@
         <v>21.6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1063,10 +1185,10 @@
         <v>21.1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1074,10 +1196,10 @@
         <v>20.7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1085,10 +1207,10 @@
         <v>20.2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1096,10 +1218,10 @@
         <v>19.8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1107,10 +1229,10 @@
         <v>19.3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1118,10 +1240,10 @@
         <v>18.899999999999999</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1129,10 +1251,10 @@
         <v>18.399999999999999</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1140,10 +1262,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1151,10 +1273,10 @@
         <v>17.600000000000001</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1162,13 +1284,14 @@
         <v>17.2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1179,45 +1302,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="21.25" customWidth="1"/>
-    <col min="5" max="5" width="24.75" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1225,7 +1348,7 @@
         <v>20000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>550</v>
@@ -1237,7 +1360,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1245,7 +1368,7 @@
         <v>13000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>850</v>
@@ -1257,7 +1380,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1265,7 +1388,7 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1150</v>
@@ -1277,7 +1400,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1285,7 +1408,7 @@
         <v>8200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>1450</v>
@@ -1297,7 +1420,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1305,7 +1428,7 @@
         <v>6800</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>1750</v>
@@ -1317,7 +1440,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1325,7 +1448,7 @@
         <v>5900</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>2050</v>
@@ -1337,7 +1460,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1345,7 +1468,7 @@
         <v>5200</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>2350</v>
@@ -1357,7 +1480,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1365,7 +1488,7 @@
         <v>4600</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>2650</v>
@@ -1377,7 +1500,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1385,7 +1508,7 @@
         <v>4120</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>550</v>
@@ -1397,7 +1520,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1405,7 +1528,7 @@
         <v>3750</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>850</v>
@@ -1417,7 +1540,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1425,7 +1548,7 @@
         <v>3400</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>1150</v>
@@ -1437,7 +1560,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1445,7 +1568,7 @@
         <v>3200</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>1450</v>
@@ -1457,7 +1580,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1465,7 +1588,7 @@
         <v>2940</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>1750</v>
@@ -1477,7 +1600,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1485,7 +1608,7 @@
         <v>2740</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>2050</v>
@@ -1497,7 +1620,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1505,7 +1628,7 @@
         <v>2600</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>2350</v>
@@ -1517,7 +1640,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1525,7 +1648,7 @@
         <v>2410</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>2650</v>
@@ -1537,7 +1660,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1545,7 +1668,7 @@
         <v>2300</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>550</v>
@@ -1557,7 +1680,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1565,7 +1688,7 @@
         <v>2150</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>850</v>
@@ -1577,7 +1700,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1585,7 +1708,7 @@
         <v>2050</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>1150</v>
@@ -1597,7 +1720,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1605,7 +1728,7 @@
         <v>1960</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>1450</v>
@@ -1617,7 +1740,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1625,7 +1748,7 @@
         <v>1870</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>1750</v>
@@ -1637,7 +1760,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1645,7 +1768,7 @@
         <v>1780</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>2050</v>
@@ -1657,7 +1780,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1665,7 +1788,7 @@
         <v>1700</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <v>2350</v>
@@ -1677,7 +1800,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1685,7 +1808,7 @@
         <v>1640</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D25">
         <v>2650</v>
@@ -1697,7 +1820,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1705,7 +1828,7 @@
         <v>1560</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>550</v>
@@ -1717,7 +1840,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1725,7 +1848,7 @@
         <v>1500</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D27">
         <v>850</v>
@@ -1737,7 +1860,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1745,7 +1868,7 @@
         <v>1450</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>1150</v>
@@ -1757,7 +1880,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1765,7 +1888,7 @@
         <v>1400</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D29">
         <v>1450</v>
@@ -1777,7 +1900,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1785,7 +1908,7 @@
         <v>1350</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>1750</v>
@@ -1797,7 +1920,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1805,7 +1928,7 @@
         <v>1300</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D31">
         <v>2050</v>
@@ -1817,7 +1940,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1825,7 +1948,7 @@
         <v>1260</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D32">
         <v>2350</v>
@@ -1837,7 +1960,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1845,7 +1968,7 @@
         <v>1220</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>2650</v>
@@ -1857,7 +1980,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1865,7 +1988,7 @@
         <v>1180</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D34">
         <v>550</v>
@@ -1877,7 +2000,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1885,7 +2008,7 @@
         <v>1150</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>850</v>
@@ -1897,7 +2020,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1905,7 +2028,7 @@
         <v>1120</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>1150</v>
@@ -1917,7 +2040,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1925,7 +2048,7 @@
         <v>1090</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D37">
         <v>1450</v>
@@ -1937,7 +2060,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1945,7 +2068,7 @@
         <v>1060</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D38">
         <v>1750</v>
@@ -1957,7 +2080,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1965,7 +2088,7 @@
         <v>1024</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D39">
         <v>2050</v>
@@ -1977,7 +2100,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1985,7 +2108,7 @@
         <v>1000</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D40">
         <v>2350</v>
@@ -1997,7 +2120,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2005,7 +2128,7 @@
         <v>976</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D41">
         <v>2650</v>
@@ -2017,7 +2140,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2025,7 +2148,7 @@
         <v>953</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D42">
         <v>550</v>
@@ -2037,7 +2160,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2045,7 +2168,7 @@
         <v>931</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>850</v>
@@ -2057,7 +2180,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2065,7 +2188,7 @@
         <v>909</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D44">
         <v>1150</v>
@@ -2077,7 +2200,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2085,7 +2208,7 @@
         <v>887</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D45">
         <v>1450</v>
@@ -2097,7 +2220,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2105,7 +2228,7 @@
         <v>866</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>1750</v>
@@ -2117,7 +2240,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2125,7 +2248,7 @@
         <v>846</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D47">
         <v>2050</v>
@@ -2137,7 +2260,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2145,7 +2268,7 @@
         <v>825</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>2350</v>
@@ -2157,7 +2280,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2165,7 +2288,7 @@
         <v>808</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D49">
         <v>2650</v>
@@ -2177,7 +2300,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2185,7 +2308,7 @@
         <v>790</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D50">
         <v>550</v>
@@ -2197,7 +2320,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2205,7 +2328,7 @@
         <v>777</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D51">
         <v>850</v>
@@ -2217,7 +2340,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2225,7 +2348,7 @@
         <v>760</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D52">
         <v>1150</v>
@@ -2237,7 +2360,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2245,7 +2368,7 @@
         <v>741</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D53">
         <v>1450</v>
@@ -2257,7 +2380,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2265,7 +2388,7 @@
         <v>732</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D54">
         <v>1750</v>
@@ -2277,7 +2400,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2285,7 +2408,7 @@
         <v>715</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D55">
         <v>2050</v>
@@ -2297,7 +2420,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2305,7 +2428,7 @@
         <v>700</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D56">
         <v>2350</v>
@@ -2317,7 +2440,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2325,7 +2448,7 @@
         <v>689</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D57">
         <v>2650</v>
@@ -2337,7 +2460,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2345,7 +2468,7 @@
         <v>676</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D58">
         <v>550</v>
@@ -2357,7 +2480,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2365,7 +2488,7 @@
         <v>665</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D59">
         <v>850</v>
@@ -2377,7 +2500,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2385,7 +2508,7 @@
         <v>652</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D60">
         <v>1150</v>
@@ -2397,7 +2520,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2405,7 +2528,7 @@
         <v>640</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D61">
         <v>1450</v>
@@ -2417,7 +2540,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2425,7 +2548,7 @@
         <v>630</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D62">
         <v>1750</v>
@@ -2437,7 +2560,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2445,7 +2568,7 @@
         <v>618</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D63">
         <v>2050</v>
@@ -2457,7 +2580,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2465,7 +2588,7 @@
         <v>609</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D64">
         <v>2350</v>
@@ -2477,7 +2600,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2485,7 +2608,7 @@
         <v>597</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D65">
         <v>2650</v>
@@ -2497,7 +2620,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2505,7 +2628,7 @@
         <v>590</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D66">
         <v>550</v>
@@ -2517,7 +2640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2525,7 +2648,7 @@
         <v>576</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D67">
         <v>850</v>
@@ -2537,7 +2660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2545,7 +2668,7 @@
         <v>569</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D68">
         <v>1150</v>
@@ -2557,7 +2680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2565,7 +2688,7 @@
         <v>560</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D69">
         <v>1450</v>
@@ -2577,7 +2700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2585,7 +2708,7 @@
         <v>550</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D70">
         <v>1750</v>
@@ -2597,7 +2720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -2605,7 +2728,7 @@
         <v>543</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D71">
         <v>2050</v>
@@ -2617,7 +2740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -2625,7 +2748,7 @@
         <v>536</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D72">
         <v>2350</v>
@@ -2637,7 +2760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -2645,7 +2768,7 @@
         <v>526</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D73">
         <v>2650</v>
@@ -2657,7 +2780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -2665,7 +2788,7 @@
         <v>520</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D74">
         <v>550</v>
@@ -2677,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -2685,7 +2808,7 @@
         <v>511</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D75">
         <v>850</v>
@@ -2697,7 +2820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2705,7 +2828,7 @@
         <v>505</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D76">
         <v>1150</v>
@@ -2717,7 +2840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -2725,7 +2848,7 @@
         <v>498</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D77">
         <v>1450</v>
@@ -2737,7 +2860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -2745,7 +2868,7 @@
         <v>490</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D78">
         <v>1750</v>
@@ -2757,7 +2880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -2765,7 +2888,7 @@
         <v>484</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D79">
         <v>2050</v>
@@ -2777,7 +2900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -2785,7 +2908,7 @@
         <v>475</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D80">
         <v>2350</v>
@@ -2797,7 +2920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -2805,7 +2928,7 @@
         <v>470</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D81">
         <v>2650</v>
@@ -2817,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -2825,7 +2948,7 @@
         <v>464</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D82">
         <v>550</v>
@@ -2837,7 +2960,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -2845,7 +2968,7 @@
         <v>457</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D83">
         <v>850</v>
@@ -2857,7 +2980,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -2865,7 +2988,7 @@
         <v>451</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D84">
         <v>1150</v>
@@ -2877,7 +3000,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -2885,7 +3008,7 @@
         <v>446</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D85">
         <v>1450</v>
@@ -2897,7 +3020,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -2905,7 +3028,7 @@
         <v>440</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D86">
         <v>1750</v>
@@ -2917,7 +3040,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -2925,7 +3048,7 @@
         <v>435</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D87">
         <v>2050</v>
@@ -2937,7 +3060,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -2945,7 +3068,7 @@
         <v>430</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D88">
         <v>2350</v>
@@ -2957,7 +3080,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2965,7 +3088,7 @@
         <v>423</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D89">
         <v>2650</v>
@@ -2977,7 +3100,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2985,7 +3108,7 @@
         <v>417</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D90">
         <v>550</v>
@@ -2997,7 +3120,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3005,7 +3128,7 @@
         <v>412</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D91">
         <v>850</v>
@@ -3017,7 +3140,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3025,7 +3148,7 @@
         <v>407</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D92">
         <v>1150</v>
@@ -3037,7 +3160,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3045,7 +3168,7 @@
         <v>402</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D93">
         <v>1450</v>
@@ -3057,7 +3180,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3065,7 +3188,7 @@
         <v>397</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D94">
         <v>1750</v>
@@ -3077,7 +3200,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3085,7 +3208,7 @@
         <v>393</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D95">
         <v>2050</v>
@@ -3097,7 +3220,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3105,7 +3228,7 @@
         <v>389</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D96">
         <v>2350</v>
@@ -3117,7 +3240,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3125,7 +3248,7 @@
         <v>385</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D97">
         <v>2650</v>
@@ -3137,7 +3260,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3145,7 +3268,7 @@
         <v>380</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D98">
         <v>550</v>
@@ -3157,7 +3280,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3165,7 +3288,7 @@
         <v>375</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D99">
         <v>850</v>
@@ -3177,7 +3300,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3185,7 +3308,7 @@
         <v>372</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D100">
         <v>1150</v>
@@ -3197,7 +3320,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3205,7 +3328,7 @@
         <v>368</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D101">
         <v>1450</v>
@@ -3217,7 +3340,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3225,7 +3348,7 @@
         <v>363</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D102">
         <v>1750</v>
@@ -3237,7 +3360,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3245,7 +3368,7 @@
         <v>360</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D103">
         <v>2050</v>
@@ -3257,7 +3380,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3265,7 +3388,7 @@
         <v>355</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D104">
         <v>2350</v>
@@ -3277,7 +3400,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3285,7 +3408,7 @@
         <v>352</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D105">
         <v>2650</v>
@@ -3297,7 +3420,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -3305,7 +3428,7 @@
         <v>348</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D106">
         <v>550</v>
@@ -3317,7 +3440,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -3325,7 +3448,7 @@
         <v>344</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D107">
         <v>850</v>
@@ -3337,7 +3460,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -3345,7 +3468,7 @@
         <v>340</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D108">
         <v>1150</v>
@@ -3357,7 +3480,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -3365,7 +3488,7 @@
         <v>336</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D109">
         <v>1450</v>
@@ -3377,7 +3500,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -3385,7 +3508,7 @@
         <v>332</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D110">
         <v>1750</v>
@@ -3397,7 +3520,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -3405,7 +3528,7 @@
         <v>330</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D111">
         <v>2050</v>
@@ -3417,7 +3540,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -3425,7 +3548,7 @@
         <v>326</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D112">
         <v>2350</v>
@@ -3437,7 +3560,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -3445,7 +3568,7 @@
         <v>323</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D113">
         <v>2650</v>
@@ -3457,7 +3580,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -3465,7 +3588,7 @@
         <v>319</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D114">
         <v>550</v>
@@ -3477,7 +3600,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -3485,7 +3608,7 @@
         <v>316</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D115">
         <v>850</v>
@@ -3497,7 +3620,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -3505,7 +3628,7 @@
         <v>313</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D116">
         <v>1150</v>
@@ -3517,7 +3640,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -3525,7 +3648,7 @@
         <v>310</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D117">
         <v>1450</v>
@@ -3537,7 +3660,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -3545,7 +3668,7 @@
         <v>307</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D118">
         <v>1750</v>
@@ -3557,7 +3680,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -3565,7 +3688,7 @@
         <v>304</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D119">
         <v>2050</v>
@@ -3577,7 +3700,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -3585,7 +3708,7 @@
         <v>301</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D120">
         <v>2350</v>
@@ -3597,7 +3720,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -3605,7 +3728,7 @@
         <v>298</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D121">
         <v>2650</v>
@@ -3617,7 +3740,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -3625,7 +3748,7 @@
         <v>295</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D122">
         <v>550</v>
@@ -3637,7 +3760,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -3645,7 +3768,7 @@
         <v>292</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D123">
         <v>850</v>
@@ -3657,7 +3780,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -3665,7 +3788,7 @@
         <v>290</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D124">
         <v>1150</v>
@@ -3677,7 +3800,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -3685,7 +3808,7 @@
         <v>287</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D125">
         <v>1450</v>
@@ -3697,7 +3820,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -3705,7 +3828,7 @@
         <v>284</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D126">
         <v>1750</v>
@@ -3717,7 +3840,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -3725,7 +3848,7 @@
         <v>282</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D127">
         <v>2050</v>
@@ -3737,7 +3860,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -3745,7 +3868,7 @@
         <v>279</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D128">
         <v>2350</v>
@@ -3757,7 +3880,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -3765,7 +3888,7 @@
         <v>277</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D129">
         <v>2650</v>

</xml_diff>